<commit_message>
- Close points form 2 till 6 - Open points 7 and 8
Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="CYRS review" sheetId="4" r:id="rId1"/>
+    <sheet name="SRS review" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>Review point</t>
   </si>
@@ -164,12 +164,24 @@
       <t xml:space="preserve"> to explicitely state that the software design should follow the described flow chart .</t>
     </r>
   </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>13/2/2020</t>
+  </si>
+  <si>
+    <t>Tones that will be sent to buzzer aren't defined, For example the tone signal is DC signal or PWM and if it's PWM what's the duty and freq. for it?</t>
+  </si>
+  <si>
+    <t>Cur_x and Cur_y are not deined with specific values, developer shall know the exact values for them</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,7 +251,179 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -339,7 +523,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,10 +555,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,7 +589,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -582,24 +764,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -622,7 +804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="5">
         <v>43984</v>
       </c>
@@ -639,13 +821,13 @@
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="75">
       <c r="A3" s="5">
         <v>43984</v>
       </c>
@@ -662,13 +844,13 @@
         <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="60">
       <c r="A4" s="5">
         <v>43984</v>
       </c>
@@ -685,13 +867,13 @@
         <v>15</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45">
       <c r="A5" s="5">
         <v>43984</v>
       </c>
@@ -708,13 +890,13 @@
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75">
       <c r="A6" s="5">
         <v>43984</v>
       </c>
@@ -731,91 +913,115 @@
         <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="45">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
@@ -823,29 +1029,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F6 G4">
-    <cfRule type="containsText" dxfId="4" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="24" priority="38" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="23" priority="39" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="22" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated the Review sheet of the SRS document
Updated the comment on the review point ragrading the buzzer tones
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -10,12 +10,11 @@
     <sheet name="SRS review" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Review point</t>
   </si>
@@ -268,7 +267,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">This relevant questions in the SIQ document are: </t>
+      <t xml:space="preserve">Updated the requirements </t>
     </r>
     <r>
       <rPr>
@@ -279,17 +278,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>PO1_DGC_SIQ_006</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
+      <t>Req_PO1_DGC_SRS_004_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
     </r>
     <r>
       <rPr>
@@ -300,60 +299,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>PO1_DGC_SIQ_007</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PO1_DGC_SIQ_008</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>PO1_DGC_SIQ_009</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-But they were not answered, please check them out.</t>
+      <t>Req_PO1_DGC_SRS_005_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to reflect the new requirements.</t>
     </r>
   </si>
 </sst>
@@ -863,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1028,7 +984,9 @@
       <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Update point 7 and 8 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="SRS review" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Review point</t>
   </si>
@@ -174,7 +174,54 @@
     <t>Tones that will be sent to buzzer aren't defined, For example the tone signal is DC signal or PWM and if it's PWM what's the duty and freq. for it?</t>
   </si>
   <si>
-    <t>Cur_x and Cur_y are not deined with specific values, developer shall know the exact values for them</t>
+    <r>
+      <t xml:space="preserve">Updated the requirements </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_004_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_005_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to reflect the new requirements.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cur_x and Cur_y are not defined with specific values, developer shall know the exact values for them</t>
   </si>
   <si>
     <r>
@@ -262,62 +309,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> to indicate the ranges of the horizontal and vertical cursor positions and what should happen if they were exceeded</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Updated the requirements </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Req_PO1_DGC_SRS_004_V01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Req_PO1_DGC_SRS_005_V01</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to reflect the new requirements.</t>
+      <t xml:space="preserve"> to indicate the ranges of the horizontal and vertical cursor positions and what should happen if they were exceeded
+Mali 19/2/2020: I didn't mean that, I meant for example Req_PO1_DGC_SRS_009_V01 the requirement shall mention the value of x and y</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +574,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -605,10 +606,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,7 +640,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -816,24 +815,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -856,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="5">
         <v>43984</v>
       </c>
@@ -879,7 +878,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="75">
       <c r="A3" s="5">
         <v>43984</v>
       </c>
@@ -902,7 +901,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="60">
       <c r="A4" s="5">
         <v>43984</v>
       </c>
@@ -925,7 +924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45">
       <c r="A5" s="5">
         <v>43984</v>
       </c>
@@ -948,7 +947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75">
       <c r="A6" s="5">
         <v>43984</v>
       </c>
@@ -971,7 +970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="60">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -988,13 +987,13 @@
         <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="165">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -1005,85 +1004,83 @@
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>

</xml_diff>

<commit_message>
Updated SRS document to V1.6
Updated SRS requirements Req_PO1_DGC_SRS_014_V01 and Req_PO1_DGC_SRS_016_V01 to be more descriptive regarding the indicators of the cursor position
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="SRS review" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Review point</t>
   </si>
@@ -310,15 +310,58 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> to indicate the ranges of the horizontal and vertical cursor positions and what should happen if they were exceeded
-Mali 19/2/2020: I didn't mean that, I meant for example Req_PO1_DGC_SRS_009_V01 the requirement shall mention the value of x and y</t>
+Mali 19/2/2020: I didn't mean that, I meant for example Req_PO1_DGC_SRS_009_V01 the requirement shall mention the value of x and y
+Mina 20/02/2020: The values cannot be mentioned exactly/explicitly since they're a range. But the requirements </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_014_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_016_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> were updated to be more descriptive.</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,7 +617,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -606,9 +649,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -640,6 +684,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -815,24 +860,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.88671875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -855,7 +900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>43984</v>
       </c>
@@ -878,7 +923,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="75">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>43984</v>
       </c>
@@ -901,7 +946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60">
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>43984</v>
       </c>
@@ -924,7 +969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43984</v>
       </c>
@@ -947,7 +992,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>43984</v>
       </c>
@@ -970,7 +1015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60">
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -993,7 +1038,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="165">
+    <row r="8" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -1006,7 +1051,9 @@
       <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1014,73 +1061,73 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>

</xml_diff>

<commit_message>
Update points 8,9 and 10 Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="SRS review" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Review point</t>
   </si>
@@ -355,13 +355,23 @@
       </rPr>
       <t xml:space="preserve"> were updated to be more descriptive.</t>
     </r>
+  </si>
+  <si>
+    <t>24/2/2020</t>
+  </si>
+  <si>
+    <t>Move SRS context under project description</t>
+  </si>
+  <si>
+    <t>SRS context shall not has a req_ID remove it's presence form 
+SRS_013, alos inputs and outputs have no meaning for this requirement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,11 +437,189 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -617,7 +805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -649,10 +837,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -684,7 +871,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -860,24 +1046,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -900,7 +1086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30">
       <c r="A2" s="5">
         <v>43984</v>
       </c>
@@ -923,7 +1109,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="75">
       <c r="A3" s="5">
         <v>43984</v>
       </c>
@@ -946,7 +1132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="60">
       <c r="A4" s="5">
         <v>43984</v>
       </c>
@@ -969,7 +1155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45">
       <c r="A5" s="5">
         <v>43984</v>
       </c>
@@ -992,7 +1178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="75">
       <c r="A6" s="5">
         <v>43984</v>
       </c>
@@ -1015,7 +1201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="60">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
@@ -1038,7 +1224,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="255">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
@@ -1055,79 +1241,103 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
@@ -1135,67 +1345,105 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F6 G4">
-    <cfRule type="containsText" dxfId="14" priority="38" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="34" priority="48" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="39" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="33" priority="49" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="40" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="32" priority="50" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="28" priority="19" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="20" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="containsText" dxfId="9" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into SRS_branch"
This reverts commit f1c01c9b97244ac22ca8120d954ebc5448b6d048, reversing
changes made to d9b955a553ed0defed4d8408a6fb93119c77dca5.
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Review point</t>
   </si>
@@ -355,26 +355,6 @@
       </rPr>
       <t xml:space="preserve"> were updated to be more descriptive.</t>
     </r>
-  </si>
-  <si>
-    <t>24/2/2020</t>
-  </si>
-  <si>
-    <t>Move SRS context under project description</t>
-  </si>
-  <si>
-    <t>SRS context shall not has a req_ID remove it's presence form 
-SRS_013, alos inputs and outputs have no meaning for this requirement</t>
-  </si>
-  <si>
-    <t>28/2/2020</t>
-  </si>
-  <si>
-    <t>Alzahraa</t>
-  </si>
-  <si>
-    <t>Req_PO1_DGC_SRS_001_V01:
-Requirement shall be splitted into 2 requirements, one for accepting input op1, op2 and operator, and another for calculating result</t>
   </si>
 </sst>
 </file>
@@ -418,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -447,127 +427,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <condense val="0"/>
@@ -999,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,65 +1055,29 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
@@ -1307,116 +1135,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F6 G4">
-    <cfRule type="containsText" dxfId="27" priority="51" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="14" priority="38" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="52" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="13" priority="39" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="53" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="12" priority="40" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",F9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"Accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",F10)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"Rejected"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>"Accepted"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",F11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' into SRS_branch""
This reverts commit 4e95132b2f1ab0a54276e42e35cfec376d50663d.
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
   <si>
     <t>Review point</t>
   </si>
@@ -355,6 +355,26 @@
       </rPr>
       <t xml:space="preserve"> were updated to be more descriptive.</t>
     </r>
+  </si>
+  <si>
+    <t>24/2/2020</t>
+  </si>
+  <si>
+    <t>Move SRS context under project description</t>
+  </si>
+  <si>
+    <t>SRS context shall not has a req_ID remove it's presence form 
+SRS_013, alos inputs and outputs have no meaning for this requirement</t>
+  </si>
+  <si>
+    <t>28/2/2020</t>
+  </si>
+  <si>
+    <t>Alzahraa</t>
+  </si>
+  <si>
+    <t>Req_PO1_DGC_SRS_001_V01:
+Requirement shall be splitted into 2 requirements, one for accepting input op1, op2 and operator, and another for calculating result</t>
   </si>
 </sst>
 </file>
@@ -398,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,11 +447,127 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -863,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1055,29 +1191,65 @@
         <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
@@ -1135,67 +1307,116 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F6 G4">
-    <cfRule type="containsText" dxfId="14" priority="38" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="51" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="39" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="26" priority="52" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="40" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="25" priority="53" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated SRS document to V1.9
Updated Req_PO1_DGC_SRS_001_V01 to be more atomic/specific, and only concerned with operands 1 and 2, and the operator
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Review point</t>
   </si>
@@ -375,6 +375,83 @@
   <si>
     <t>Req_PO1_DGC_SRS_001_V01:
 Requirement shall be splitted into 2 requirements, one for accepting input op1, op2 and operator, and another for calculating result</t>
+  </si>
+  <si>
+    <t>Moved the Context diagram under the project description</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reverted back </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_013_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to its original state, which idicates that the software design should follow the Flow Chart</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Made </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_001_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> more specific and only concerned with operands 1 and 2, and the operator.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_018_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is already concerened with storing/calculatung the result.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -999,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1210,9 +1287,14 @@
       <c r="D9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1228,12 +1310,17 @@
       <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G10" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1246,9 +1333,14 @@
       <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1393,7 +1485,7 @@
       <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="E10:E11">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
@@ -1416,7 +1508,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated SRS document to V1.9 (#28)
* Updated SRS to V1.7

- Added Table of signals

- Added Context diagram

- Categorized requirements

- Fixed some typos

* Revert "Merge branch 'master' into SRS_branch"

This reverts commit f1c01c9b97244ac22ca8120d954ebc5448b6d048, reversing
changes made to d9b955a553ed0defed4d8408a6fb93119c77dca5.

* Revert "Revert "Merge branch 'master' into SRS_branch""

This reverts commit 4e95132b2f1ab0a54276e42e35cfec376d50663d.

* Updated SRS document to V1.9

Updated Req_PO1_DGC_SRS_001_V01 to be more atomic/specific, and only concerned with operands 1 and 2, and the operator
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/Review.xlsx
+++ b/Software Specification/SRS/Review.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
   <si>
     <t>Review point</t>
   </si>
@@ -375,6 +375,83 @@
   <si>
     <t>Req_PO1_DGC_SRS_001_V01:
 Requirement shall be splitted into 2 requirements, one for accepting input op1, op2 and operator, and another for calculating result</t>
+  </si>
+  <si>
+    <t>Moved the Context diagram under the project description</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reverted back </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_013_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to its original state, which idicates that the software design should follow the Flow Chart</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Made </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_001_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> more specific and only concerned with operands 1 and 2, and the operator.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_PO1_DGC_SRS_018_V01</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is already concerened with storing/calculatung the result.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -999,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1210,9 +1287,14 @@
       <c r="D9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -1228,12 +1310,17 @@
       <c r="D10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G10" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1246,9 +1333,14 @@
       <c r="D11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1393,7 +1485,7 @@
       <formula>NOT(ISERROR(SEARCH("Open",F10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
+  <conditionalFormatting sqref="E10:E11">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
@@ -1416,7 +1508,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F11">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>